<commit_message>
AP: dy_qt data CMS
</commit_message>
<xml_diff>
--- a/dy_qT/expdata/10001.xlsx
+++ b/dy_qT/expdata/10001.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avp5627/GIT/fitpack2/database/z_qT/expdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avp5627/GIT/fitpack2/database/dy_qT/expdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9E8B3A-DB11-DC40-9872-6D18BA32E995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5E974B-3160-F846-9265-9A1E76641D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3060" yWindow="2480" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="29">
   <si>
     <t>FiducialCuts</t>
   </si>
@@ -40,12 +40,6 @@
   </si>
   <si>
     <t>etaMax</t>
-  </si>
-  <si>
-    <t>stat_plus</t>
-  </si>
-  <si>
-    <t>stat_minus</t>
   </si>
   <si>
     <t>Q</t>
@@ -99,12 +93,6 @@
     <t>1/GeV</t>
   </si>
   <si>
-    <t>%syst_c</t>
-  </si>
-  <si>
-    <t>stat_u</t>
-  </si>
-  <si>
     <t>beam</t>
   </si>
   <si>
@@ -121,6 +109,15 @@
   </si>
   <si>
     <t>pp-&gt;Z/gamma*-&gt;l+ l-</t>
+  </si>
+  <si>
+    <t>tot_u</t>
+  </si>
+  <si>
+    <t>tot_plus</t>
+  </si>
+  <si>
+    <t>tot_minus</t>
   </si>
 </sst>
 </file>
@@ -970,92 +967,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y35"/>
+  <dimension ref="A1:X35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AB35" sqref="AB35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
-      </c>
-      <c r="L1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R1" t="s">
-        <v>1</v>
-      </c>
-      <c r="S1" t="s">
-        <v>2</v>
-      </c>
-      <c r="T1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U1" t="s">
-        <v>14</v>
       </c>
       <c r="V1" t="s">
         <v>20</v>
       </c>
       <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
         <v>24</v>
       </c>
-      <c r="X1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>SQRT(169000000)</f>
         <v>13000</v>
@@ -1100,20 +1094,20 @@
       <c r="N2">
         <v>-2.6898999999999998E-4</v>
       </c>
-      <c r="O2">
-        <v>2.5</v>
-      </c>
-      <c r="P2" t="b">
+      <c r="O2" t="b">
         <v>1</v>
       </c>
+      <c r="P2">
+        <v>25</v>
+      </c>
       <c r="Q2">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R2">
-        <v>-2.4</v>
-      </c>
-      <c r="S2">
         <v>2.4</v>
+      </c>
+      <c r="S2" t="s">
+        <v>15</v>
       </c>
       <c r="T2" t="s">
         <v>17</v>
@@ -1125,16 +1119,13 @@
         <v>21</v>
       </c>
       <c r="W2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X2" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>SQRT(169000000)</f>
         <v>13000</v>
@@ -1179,20 +1170,20 @@
       <c r="N3">
         <v>-6.7723000000000002E-4</v>
       </c>
-      <c r="O3">
-        <v>2.5</v>
-      </c>
-      <c r="P3" t="b">
+      <c r="O3" t="b">
         <v>1</v>
       </c>
+      <c r="P3">
+        <v>25</v>
+      </c>
       <c r="Q3">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R3">
-        <v>-2.4</v>
-      </c>
-      <c r="S3">
         <v>2.4</v>
+      </c>
+      <c r="S3" t="s">
+        <v>15</v>
       </c>
       <c r="T3" t="s">
         <v>17</v>
@@ -1204,16 +1195,13 @@
         <v>21</v>
       </c>
       <c r="W3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X3" t="s">
         <v>25</v>
       </c>
-      <c r="Y3" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A35" si="1">SQRT(169000000)</f>
         <v>13000</v>
@@ -1258,20 +1246,20 @@
       <c r="N4">
         <v>-9.1755000000000005E-4</v>
       </c>
-      <c r="O4">
-        <v>2.5</v>
-      </c>
-      <c r="P4" t="b">
+      <c r="O4" t="b">
         <v>1</v>
       </c>
+      <c r="P4">
+        <v>25</v>
+      </c>
       <c r="Q4">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R4">
-        <v>-2.4</v>
-      </c>
-      <c r="S4">
         <v>2.4</v>
+      </c>
+      <c r="S4" t="s">
+        <v>15</v>
       </c>
       <c r="T4" t="s">
         <v>17</v>
@@ -1283,16 +1271,13 @@
         <v>21</v>
       </c>
       <c r="W4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X4" t="s">
         <v>25</v>
       </c>
-      <c r="Y4" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1337,20 +1322,20 @@
       <c r="N5">
         <v>-9.7210000000000005E-4</v>
       </c>
-      <c r="O5">
-        <v>2.5</v>
-      </c>
-      <c r="P5" t="b">
+      <c r="O5" t="b">
         <v>1</v>
       </c>
+      <c r="P5">
+        <v>25</v>
+      </c>
       <c r="Q5">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R5">
-        <v>-2.4</v>
-      </c>
-      <c r="S5">
         <v>2.4</v>
+      </c>
+      <c r="S5" t="s">
+        <v>15</v>
       </c>
       <c r="T5" t="s">
         <v>17</v>
@@ -1362,16 +1347,13 @@
         <v>21</v>
       </c>
       <c r="W5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X5" t="s">
         <v>25</v>
       </c>
-      <c r="Y5" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1416,20 +1398,20 @@
       <c r="N6">
         <v>-9.5901999999999999E-4</v>
       </c>
-      <c r="O6">
-        <v>2.5</v>
-      </c>
-      <c r="P6" t="b">
+      <c r="O6" t="b">
         <v>1</v>
       </c>
+      <c r="P6">
+        <v>25</v>
+      </c>
       <c r="Q6">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R6">
-        <v>-2.4</v>
-      </c>
-      <c r="S6">
         <v>2.4</v>
+      </c>
+      <c r="S6" t="s">
+        <v>15</v>
       </c>
       <c r="T6" t="s">
         <v>17</v>
@@ -1441,16 +1423,13 @@
         <v>21</v>
       </c>
       <c r="W6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X6" t="s">
         <v>25</v>
       </c>
-      <c r="Y6" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1495,20 +1474,20 @@
       <c r="N7">
         <v>-9.2347999999999996E-4</v>
       </c>
-      <c r="O7">
-        <v>2.5</v>
-      </c>
-      <c r="P7" t="b">
+      <c r="O7" t="b">
         <v>1</v>
       </c>
+      <c r="P7">
+        <v>25</v>
+      </c>
       <c r="Q7">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R7">
-        <v>-2.4</v>
-      </c>
-      <c r="S7">
         <v>2.4</v>
+      </c>
+      <c r="S7" t="s">
+        <v>15</v>
       </c>
       <c r="T7" t="s">
         <v>17</v>
@@ -1520,16 +1499,13 @@
         <v>21</v>
       </c>
       <c r="W7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X7" t="s">
         <v>25</v>
       </c>
-      <c r="Y7" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1574,20 +1550,20 @@
       <c r="N8">
         <v>-8.7613999999999997E-4</v>
       </c>
-      <c r="O8">
-        <v>2.5</v>
-      </c>
-      <c r="P8" t="b">
+      <c r="O8" t="b">
         <v>1</v>
       </c>
+      <c r="P8">
+        <v>25</v>
+      </c>
       <c r="Q8">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R8">
-        <v>-2.4</v>
-      </c>
-      <c r="S8">
         <v>2.4</v>
+      </c>
+      <c r="S8" t="s">
+        <v>15</v>
       </c>
       <c r="T8" t="s">
         <v>17</v>
@@ -1599,16 +1575,13 @@
         <v>21</v>
       </c>
       <c r="W8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X8" t="s">
         <v>25</v>
       </c>
-      <c r="Y8" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1653,20 +1626,20 @@
       <c r="N9">
         <v>-8.273E-4</v>
       </c>
-      <c r="O9">
-        <v>2.5</v>
-      </c>
-      <c r="P9" t="b">
+      <c r="O9" t="b">
         <v>1</v>
       </c>
+      <c r="P9">
+        <v>25</v>
+      </c>
       <c r="Q9">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R9">
-        <v>-2.4</v>
-      </c>
-      <c r="S9">
         <v>2.4</v>
+      </c>
+      <c r="S9" t="s">
+        <v>15</v>
       </c>
       <c r="T9" t="s">
         <v>17</v>
@@ -1678,16 +1651,13 @@
         <v>21</v>
       </c>
       <c r="W9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X9" t="s">
         <v>25</v>
       </c>
-      <c r="Y9" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1732,20 +1702,20 @@
       <c r="N10">
         <v>-7.7424000000000004E-4</v>
       </c>
-      <c r="O10">
-        <v>2.5</v>
-      </c>
-      <c r="P10" t="b">
+      <c r="O10" t="b">
         <v>1</v>
       </c>
+      <c r="P10">
+        <v>25</v>
+      </c>
       <c r="Q10">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R10">
-        <v>-2.4</v>
-      </c>
-      <c r="S10">
         <v>2.4</v>
+      </c>
+      <c r="S10" t="s">
+        <v>15</v>
       </c>
       <c r="T10" t="s">
         <v>17</v>
@@ -1757,16 +1727,13 @@
         <v>21</v>
       </c>
       <c r="W10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X10" t="s">
         <v>25</v>
       </c>
-      <c r="Y10" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1811,20 +1778,20 @@
       <c r="N11">
         <v>-7.0032999999999998E-4</v>
       </c>
-      <c r="O11">
-        <v>2.5</v>
-      </c>
-      <c r="P11" t="b">
+      <c r="O11" t="b">
         <v>1</v>
       </c>
+      <c r="P11">
+        <v>25</v>
+      </c>
       <c r="Q11">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R11">
-        <v>-2.4</v>
-      </c>
-      <c r="S11">
         <v>2.4</v>
+      </c>
+      <c r="S11" t="s">
+        <v>15</v>
       </c>
       <c r="T11" t="s">
         <v>17</v>
@@ -1836,16 +1803,13 @@
         <v>21</v>
       </c>
       <c r="W11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X11" t="s">
         <v>25</v>
       </c>
-      <c r="Y11" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1890,20 +1854,20 @@
       <c r="N12">
         <v>-6.2615000000000001E-4</v>
       </c>
-      <c r="O12">
-        <v>2.5</v>
-      </c>
-      <c r="P12" t="b">
+      <c r="O12" t="b">
         <v>1</v>
       </c>
+      <c r="P12">
+        <v>25</v>
+      </c>
       <c r="Q12">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R12">
-        <v>-2.4</v>
-      </c>
-      <c r="S12">
         <v>2.4</v>
+      </c>
+      <c r="S12" t="s">
+        <v>15</v>
       </c>
       <c r="T12" t="s">
         <v>17</v>
@@ -1915,16 +1879,13 @@
         <v>21</v>
       </c>
       <c r="W12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X12" t="s">
         <v>25</v>
       </c>
-      <c r="Y12" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -1969,20 +1930,20 @@
       <c r="N13">
         <v>-5.6835000000000002E-4</v>
       </c>
-      <c r="O13">
-        <v>2.5</v>
-      </c>
-      <c r="P13" t="b">
+      <c r="O13" t="b">
         <v>1</v>
       </c>
+      <c r="P13">
+        <v>25</v>
+      </c>
       <c r="Q13">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R13">
-        <v>-2.4</v>
-      </c>
-      <c r="S13">
         <v>2.4</v>
+      </c>
+      <c r="S13" t="s">
+        <v>15</v>
       </c>
       <c r="T13" t="s">
         <v>17</v>
@@ -1994,16 +1955,13 @@
         <v>21</v>
       </c>
       <c r="W13" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X13" t="s">
         <v>25</v>
       </c>
-      <c r="Y13" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2048,20 +2006,20 @@
       <c r="N14">
         <v>-5.3012000000000003E-4</v>
       </c>
-      <c r="O14">
-        <v>2.5</v>
-      </c>
-      <c r="P14" t="b">
+      <c r="O14" t="b">
         <v>1</v>
       </c>
+      <c r="P14">
+        <v>25</v>
+      </c>
       <c r="Q14">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R14">
-        <v>-2.4</v>
-      </c>
-      <c r="S14">
         <v>2.4</v>
+      </c>
+      <c r="S14" t="s">
+        <v>15</v>
       </c>
       <c r="T14" t="s">
         <v>17</v>
@@ -2073,16 +2031,13 @@
         <v>21</v>
       </c>
       <c r="W14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X14" t="s">
         <v>25</v>
       </c>
-      <c r="Y14" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2127,20 +2082,20 @@
       <c r="N15">
         <v>-4.8897000000000003E-4</v>
       </c>
-      <c r="O15">
-        <v>2.5</v>
-      </c>
-      <c r="P15" t="b">
+      <c r="O15" t="b">
         <v>1</v>
       </c>
+      <c r="P15">
+        <v>25</v>
+      </c>
       <c r="Q15">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R15">
-        <v>-2.4</v>
-      </c>
-      <c r="S15">
         <v>2.4</v>
+      </c>
+      <c r="S15" t="s">
+        <v>15</v>
       </c>
       <c r="T15" t="s">
         <v>17</v>
@@ -2152,16 +2107,13 @@
         <v>21</v>
       </c>
       <c r="W15" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X15" t="s">
         <v>25</v>
       </c>
-      <c r="Y15" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2206,20 +2158,20 @@
       <c r="N16">
         <v>-4.2590999999999999E-4</v>
       </c>
-      <c r="O16">
-        <v>2.5</v>
-      </c>
-      <c r="P16" t="b">
+      <c r="O16" t="b">
         <v>1</v>
       </c>
+      <c r="P16">
+        <v>25</v>
+      </c>
       <c r="Q16">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R16">
-        <v>-2.4</v>
-      </c>
-      <c r="S16">
         <v>2.4</v>
+      </c>
+      <c r="S16" t="s">
+        <v>15</v>
       </c>
       <c r="T16" t="s">
         <v>17</v>
@@ -2231,16 +2183,13 @@
         <v>21</v>
       </c>
       <c r="W16" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X16" t="s">
         <v>25</v>
       </c>
-      <c r="Y16" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2285,20 +2234,20 @@
       <c r="N17">
         <v>-3.6234E-4</v>
       </c>
-      <c r="O17">
-        <v>2.5</v>
-      </c>
-      <c r="P17" t="b">
+      <c r="O17" t="b">
         <v>1</v>
       </c>
+      <c r="P17">
+        <v>25</v>
+      </c>
       <c r="Q17">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R17">
-        <v>-2.4</v>
-      </c>
-      <c r="S17">
         <v>2.4</v>
+      </c>
+      <c r="S17" t="s">
+        <v>15</v>
       </c>
       <c r="T17" t="s">
         <v>17</v>
@@ -2310,16 +2259,13 @@
         <v>21</v>
       </c>
       <c r="W17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X17" t="s">
         <v>25</v>
       </c>
-      <c r="Y17" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2364,20 +2310,20 @@
       <c r="N18">
         <v>-3.1348999999999998E-4</v>
       </c>
-      <c r="O18">
-        <v>2.5</v>
-      </c>
-      <c r="P18" t="b">
+      <c r="O18" t="b">
         <v>1</v>
       </c>
+      <c r="P18">
+        <v>25</v>
+      </c>
       <c r="Q18">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R18">
-        <v>-2.4</v>
-      </c>
-      <c r="S18">
         <v>2.4</v>
+      </c>
+      <c r="S18" t="s">
+        <v>15</v>
       </c>
       <c r="T18" t="s">
         <v>17</v>
@@ -2389,16 +2335,13 @@
         <v>21</v>
       </c>
       <c r="W18" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X18" t="s">
         <v>25</v>
       </c>
-      <c r="Y18" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2443,20 +2386,20 @@
       <c r="N19">
         <v>-2.6678999999999999E-4</v>
       </c>
-      <c r="O19">
-        <v>2.5</v>
-      </c>
-      <c r="P19" t="b">
+      <c r="O19" t="b">
         <v>1</v>
       </c>
+      <c r="P19">
+        <v>25</v>
+      </c>
       <c r="Q19">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R19">
-        <v>-2.4</v>
-      </c>
-      <c r="S19">
         <v>2.4</v>
+      </c>
+      <c r="S19" t="s">
+        <v>15</v>
       </c>
       <c r="T19" t="s">
         <v>17</v>
@@ -2468,16 +2411,13 @@
         <v>21</v>
       </c>
       <c r="W19" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X19" t="s">
         <v>25</v>
       </c>
-      <c r="Y19" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2522,20 +2462,20 @@
       <c r="N20">
         <v>-2.2128999999999999E-4</v>
       </c>
-      <c r="O20">
-        <v>2.5</v>
-      </c>
-      <c r="P20" t="b">
+      <c r="O20" t="b">
         <v>1</v>
       </c>
+      <c r="P20">
+        <v>25</v>
+      </c>
       <c r="Q20">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R20">
-        <v>-2.4</v>
-      </c>
-      <c r="S20">
         <v>2.4</v>
+      </c>
+      <c r="S20" t="s">
+        <v>15</v>
       </c>
       <c r="T20" t="s">
         <v>17</v>
@@ -2547,16 +2487,13 @@
         <v>21</v>
       </c>
       <c r="W20" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X20" t="s">
         <v>25</v>
       </c>
-      <c r="Y20" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2601,20 +2538,20 @@
       <c r="N21">
         <v>-1.8212999999999999E-4</v>
       </c>
-      <c r="O21">
-        <v>2.5</v>
-      </c>
-      <c r="P21" t="b">
+      <c r="O21" t="b">
         <v>1</v>
       </c>
+      <c r="P21">
+        <v>25</v>
+      </c>
       <c r="Q21">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R21">
-        <v>-2.4</v>
-      </c>
-      <c r="S21">
         <v>2.4</v>
+      </c>
+      <c r="S21" t="s">
+        <v>15</v>
       </c>
       <c r="T21" t="s">
         <v>17</v>
@@ -2626,16 +2563,13 @@
         <v>21</v>
       </c>
       <c r="W21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X21" t="s">
         <v>25</v>
       </c>
-      <c r="Y21" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2680,20 +2614,20 @@
       <c r="N22">
         <v>-1.3954000000000001E-4</v>
       </c>
-      <c r="O22">
-        <v>2.5</v>
-      </c>
-      <c r="P22" t="b">
+      <c r="O22" t="b">
         <v>1</v>
       </c>
+      <c r="P22">
+        <v>25</v>
+      </c>
       <c r="Q22">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R22">
-        <v>-2.4</v>
-      </c>
-      <c r="S22">
         <v>2.4</v>
+      </c>
+      <c r="S22" t="s">
+        <v>15</v>
       </c>
       <c r="T22" t="s">
         <v>17</v>
@@ -2705,16 +2639,13 @@
         <v>21</v>
       </c>
       <c r="W22" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X22" t="s">
         <v>25</v>
       </c>
-      <c r="Y22" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2759,20 +2690,20 @@
       <c r="N23">
         <v>-1.0692E-4</v>
       </c>
-      <c r="O23">
-        <v>2.5</v>
-      </c>
-      <c r="P23" t="b">
+      <c r="O23" t="b">
         <v>1</v>
       </c>
+      <c r="P23">
+        <v>25</v>
+      </c>
       <c r="Q23">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R23">
-        <v>-2.4</v>
-      </c>
-      <c r="S23">
         <v>2.4</v>
+      </c>
+      <c r="S23" t="s">
+        <v>15</v>
       </c>
       <c r="T23" t="s">
         <v>17</v>
@@ -2784,16 +2715,13 @@
         <v>21</v>
       </c>
       <c r="W23" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X23" t="s">
         <v>25</v>
       </c>
-      <c r="Y23" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2838,20 +2766,20 @@
       <c r="N24" s="1">
         <v>-7.8133999999999994E-5</v>
       </c>
-      <c r="O24">
-        <v>2.5</v>
-      </c>
-      <c r="P24" t="b">
+      <c r="O24" t="b">
         <v>1</v>
       </c>
+      <c r="P24">
+        <v>25</v>
+      </c>
       <c r="Q24">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R24">
-        <v>-2.4</v>
-      </c>
-      <c r="S24">
         <v>2.4</v>
+      </c>
+      <c r="S24" t="s">
+        <v>15</v>
       </c>
       <c r="T24" t="s">
         <v>17</v>
@@ -2863,16 +2791,13 @@
         <v>21</v>
       </c>
       <c r="W24" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X24" t="s">
         <v>25</v>
       </c>
-      <c r="Y24" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2917,20 +2842,20 @@
       <c r="N25" s="1">
         <v>-5.4038E-5</v>
       </c>
-      <c r="O25">
-        <v>2.5</v>
-      </c>
-      <c r="P25" t="b">
+      <c r="O25" t="b">
         <v>1</v>
       </c>
+      <c r="P25">
+        <v>25</v>
+      </c>
       <c r="Q25">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R25">
-        <v>-2.4</v>
-      </c>
-      <c r="S25">
         <v>2.4</v>
+      </c>
+      <c r="S25" t="s">
+        <v>15</v>
       </c>
       <c r="T25" t="s">
         <v>17</v>
@@ -2942,16 +2867,13 @@
         <v>21</v>
       </c>
       <c r="W25" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X25" t="s">
         <v>25</v>
       </c>
-      <c r="Y25" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -2996,20 +2918,20 @@
       <c r="N26" s="1">
         <v>-3.3306999999999998E-5</v>
       </c>
-      <c r="O26">
-        <v>2.5</v>
-      </c>
-      <c r="P26" t="b">
+      <c r="O26" t="b">
         <v>1</v>
       </c>
+      <c r="P26">
+        <v>25</v>
+      </c>
       <c r="Q26">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R26">
-        <v>-2.4</v>
-      </c>
-      <c r="S26">
         <v>2.4</v>
+      </c>
+      <c r="S26" t="s">
+        <v>15</v>
       </c>
       <c r="T26" t="s">
         <v>17</v>
@@ -3021,16 +2943,13 @@
         <v>21</v>
       </c>
       <c r="W26" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X26" t="s">
         <v>25</v>
       </c>
-      <c r="Y26" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3075,20 +2994,20 @@
       <c r="N27" s="1">
         <v>-1.8196999999999999E-5</v>
       </c>
-      <c r="O27">
-        <v>2.5</v>
-      </c>
-      <c r="P27" t="b">
+      <c r="O27" t="b">
         <v>1</v>
       </c>
+      <c r="P27">
+        <v>25</v>
+      </c>
       <c r="Q27">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R27">
-        <v>-2.4</v>
-      </c>
-      <c r="S27">
         <v>2.4</v>
+      </c>
+      <c r="S27" t="s">
+        <v>15</v>
       </c>
       <c r="T27" t="s">
         <v>17</v>
@@ -3100,16 +3019,13 @@
         <v>21</v>
       </c>
       <c r="W27" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X27" t="s">
         <v>25</v>
       </c>
-      <c r="Y27" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3154,20 +3070,20 @@
       <c r="N28" s="1">
         <v>-8.5341000000000002E-6</v>
       </c>
-      <c r="O28">
-        <v>2.5</v>
-      </c>
-      <c r="P28" t="b">
+      <c r="O28" t="b">
         <v>1</v>
       </c>
+      <c r="P28">
+        <v>25</v>
+      </c>
       <c r="Q28">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R28">
-        <v>-2.4</v>
-      </c>
-      <c r="S28">
         <v>2.4</v>
+      </c>
+      <c r="S28" t="s">
+        <v>15</v>
       </c>
       <c r="T28" t="s">
         <v>17</v>
@@ -3179,16 +3095,13 @@
         <v>21</v>
       </c>
       <c r="W28" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X28" t="s">
         <v>25</v>
       </c>
-      <c r="Y28" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3233,20 +3146,20 @@
       <c r="N29" s="1">
         <v>-3.6807000000000002E-6</v>
       </c>
-      <c r="O29">
-        <v>2.5</v>
-      </c>
-      <c r="P29" t="b">
+      <c r="O29" t="b">
         <v>1</v>
       </c>
+      <c r="P29">
+        <v>25</v>
+      </c>
       <c r="Q29">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R29">
-        <v>-2.4</v>
-      </c>
-      <c r="S29">
         <v>2.4</v>
+      </c>
+      <c r="S29" t="s">
+        <v>15</v>
       </c>
       <c r="T29" t="s">
         <v>17</v>
@@ -3258,16 +3171,13 @@
         <v>21</v>
       </c>
       <c r="W29" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X29" t="s">
         <v>25</v>
       </c>
-      <c r="Y29" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3312,20 +3222,20 @@
       <c r="N30" s="1">
         <v>-1.9126999999999999E-6</v>
       </c>
-      <c r="O30">
-        <v>2.5</v>
-      </c>
-      <c r="P30" t="b">
+      <c r="O30" t="b">
         <v>1</v>
       </c>
+      <c r="P30">
+        <v>25</v>
+      </c>
       <c r="Q30">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R30">
-        <v>-2.4</v>
-      </c>
-      <c r="S30">
         <v>2.4</v>
+      </c>
+      <c r="S30" t="s">
+        <v>15</v>
       </c>
       <c r="T30" t="s">
         <v>17</v>
@@ -3337,16 +3247,13 @@
         <v>21</v>
       </c>
       <c r="W30" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X30" t="s">
         <v>25</v>
       </c>
-      <c r="Y30" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3391,20 +3298,20 @@
       <c r="N31" s="1">
         <v>-1.2055999999999999E-6</v>
       </c>
-      <c r="O31">
-        <v>2.5</v>
-      </c>
-      <c r="P31" t="b">
+      <c r="O31" t="b">
         <v>1</v>
       </c>
+      <c r="P31">
+        <v>25</v>
+      </c>
       <c r="Q31">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R31">
-        <v>-2.4</v>
-      </c>
-      <c r="S31">
         <v>2.4</v>
+      </c>
+      <c r="S31" t="s">
+        <v>15</v>
       </c>
       <c r="T31" t="s">
         <v>17</v>
@@ -3416,16 +3323,13 @@
         <v>21</v>
       </c>
       <c r="W31" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X31" t="s">
         <v>25</v>
       </c>
-      <c r="Y31" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3470,20 +3374,20 @@
       <c r="N32" s="1">
         <v>-7.9551999999999997E-7</v>
       </c>
-      <c r="O32">
-        <v>2.5</v>
-      </c>
-      <c r="P32" t="b">
+      <c r="O32" t="b">
         <v>1</v>
       </c>
+      <c r="P32">
+        <v>25</v>
+      </c>
       <c r="Q32">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R32">
-        <v>-2.4</v>
-      </c>
-      <c r="S32">
         <v>2.4</v>
+      </c>
+      <c r="S32" t="s">
+        <v>15</v>
       </c>
       <c r="T32" t="s">
         <v>17</v>
@@ -3495,16 +3399,13 @@
         <v>21</v>
       </c>
       <c r="W32" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X32" t="s">
         <v>25</v>
       </c>
-      <c r="Y32" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3549,20 +3450,20 @@
       <c r="N33" s="1">
         <v>-4.6897E-7</v>
       </c>
-      <c r="O33">
-        <v>2.5</v>
-      </c>
-      <c r="P33" t="b">
+      <c r="O33" t="b">
         <v>1</v>
       </c>
+      <c r="P33">
+        <v>25</v>
+      </c>
       <c r="Q33">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R33">
-        <v>-2.4</v>
-      </c>
-      <c r="S33">
         <v>2.4</v>
+      </c>
+      <c r="S33" t="s">
+        <v>15</v>
       </c>
       <c r="T33" t="s">
         <v>17</v>
@@ -3574,16 +3475,13 @@
         <v>21</v>
       </c>
       <c r="W33" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X33" t="s">
         <v>25</v>
       </c>
-      <c r="Y33" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3628,20 +3526,20 @@
       <c r="N34" s="1">
         <v>-1.8589000000000001E-7</v>
       </c>
-      <c r="O34">
-        <v>2.5</v>
-      </c>
-      <c r="P34" t="b">
+      <c r="O34" t="b">
         <v>1</v>
       </c>
+      <c r="P34">
+        <v>25</v>
+      </c>
       <c r="Q34">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R34">
-        <v>-2.4</v>
-      </c>
-      <c r="S34">
         <v>2.4</v>
+      </c>
+      <c r="S34" t="s">
+        <v>15</v>
       </c>
       <c r="T34" t="s">
         <v>17</v>
@@ -3653,16 +3551,13 @@
         <v>21</v>
       </c>
       <c r="W34" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X34" t="s">
         <v>25</v>
       </c>
-      <c r="Y34" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>13000</v>
@@ -3707,20 +3602,20 @@
       <c r="N35" s="1">
         <v>-9.3459999999999998E-9</v>
       </c>
-      <c r="O35">
-        <v>2.5</v>
-      </c>
-      <c r="P35" t="b">
+      <c r="O35" t="b">
         <v>1</v>
       </c>
+      <c r="P35">
+        <v>25</v>
+      </c>
       <c r="Q35">
-        <v>25</v>
+        <v>-2.4</v>
       </c>
       <c r="R35">
-        <v>-2.4</v>
-      </c>
-      <c r="S35">
         <v>2.4</v>
+      </c>
+      <c r="S35" t="s">
+        <v>15</v>
       </c>
       <c r="T35" t="s">
         <v>17</v>
@@ -3732,13 +3627,10 @@
         <v>21</v>
       </c>
       <c r="W35" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X35" t="s">
         <v>25</v>
-      </c>
-      <c r="Y35" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>